<commit_message>
Update GeoRef und Leitfaden
</commit_message>
<xml_diff>
--- a/Doc/Priority_Trays.xlsx
+++ b/Doc/Priority_Trays.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Envimaster\DWA\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AAD4378-42C7-40A0-8D8A-23A66834E0E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC853F6C-8CE0-435B-990D-F8FDB954376C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{911DC355-DA80-4B0E-AD68-1A253E225116}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6240" xr2:uid="{911DC355-DA80-4B0E-AD68-1A253E225116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t>Roman_Nr</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Legende</t>
+  </si>
+  <si>
+    <t>GeoRef in progress</t>
+  </si>
+  <si>
+    <t>VD</t>
+  </si>
+  <si>
+    <t>JH</t>
   </si>
 </sst>
 </file>
@@ -100,12 +109,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -119,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,24 +468,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3C8B3-B0DC-4ABD-9584-533CBDE746E3}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -490,14 +502,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="5"/>
       <c r="F3" t="s">
         <v>9</v>
       </c>
@@ -505,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -520,14 +532,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
       <c r="F5" t="s">
         <v>8</v>
       </c>
@@ -535,14 +547,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
       <c r="F6" t="s">
         <v>7</v>
       </c>
@@ -550,14 +562,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
         <v>9</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="6"/>
       <c r="F7" t="s">
         <v>6</v>
       </c>
@@ -565,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -573,7 +585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -581,7 +593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -589,7 +601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -597,7 +609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -605,7 +617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -613,7 +625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -621,7 +633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -629,7 +641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -637,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -645,7 +657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -653,244 +665,310 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="6">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="5">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="5">
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="5">
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="4">
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="5">
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="3">
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="6">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="5">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="4">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B42" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="4">
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="4">
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="3">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B45" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="4">
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="3">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" s="4">
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="3">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="4">
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="3">
         <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>